<commit_message>
changes in view page
</commit_message>
<xml_diff>
--- a/wwwroot/Resume_Datas/Resume_Datas (2).xlsx
+++ b/wwwroot/Resume_Datas/Resume_Datas (2).xlsx
@@ -31,13 +31,13 @@
     <t>Skills</t>
   </si>
   <si>
-    <t>karthik</t>
-  </si>
-  <si>
-    <t>Developing</t>
-  </si>
-  <si>
-    <t>Communication</t>
+    <t>selva</t>
+  </si>
+  <si>
+    <t>coder</t>
+  </si>
+  <si>
+    <t>Absorbing</t>
   </si>
 </sst>
 </file>
@@ -319,13 +319,13 @@
         <v>6</v>
       </c>
       <c r="B2" s="1">
-        <v>436.0</v>
+        <v>400.0</v>
       </c>
       <c r="C2" s="1">
-        <v>1000.0</v>
+        <v>910.0</v>
       </c>
       <c r="D2" s="1">
-        <v>7.88</v>
+        <v>78.0</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>7</v>

</xml_diff>